<commit_message>
Added conditional formatting to output, minor code clean-up
</commit_message>
<xml_diff>
--- a/budget_report/REPORT_invoice-export-2024-12-05-08_32-jaq.xlsx
+++ b/budget_report/REPORT_invoice-export-2024-12-05-08_32-jaq.xlsx
@@ -156,7 +156,22 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -745,6 +760,14 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
   </mergeCells>
+  <conditionalFormatting sqref="B4:F15">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalized code and info box before exe generation
</commit_message>
<xml_diff>
--- a/budget_report/REPORT_invoice-export-2024-12-05-08_32-jaq.xlsx
+++ b/budget_report/REPORT_invoice-export-2024-12-05-08_32-jaq.xlsx
@@ -61,7 +61,7 @@
     <t>TOTALS</t>
   </si>
   <si>
-    <t>REPORT - CUTOFF DATE: 2025-01-29</t>
+    <t>REPORT - CUTOFF DATE: 2024-10-01</t>
   </si>
 </sst>
 </file>
@@ -475,6 +475,14 @@
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>15</v>
@@ -513,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="4">
-        <v>0</v>
+        <v>4706.24</v>
       </c>
       <c r="D4" s="4">
         <v>9130.31</v>
@@ -534,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="4">
-        <v>0</v>
+        <v>14.17</v>
       </c>
       <c r="D5" s="4">
         <v>14.17</v>
@@ -555,7 +563,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="4">
-        <v>0</v>
+        <v>419.88</v>
       </c>
       <c r="D6" s="4">
         <v>432.57</v>
@@ -597,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="4">
-        <v>0</v>
+        <v>5569.36</v>
       </c>
       <c r="D8" s="4">
         <v>10605.40</v>
@@ -639,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="4">
-        <v>0</v>
+        <v>-675.2</v>
       </c>
       <c r="D10" s="4">
         <v>100229.35</v>
@@ -660,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="4">
-        <v>0</v>
+        <v>460.48</v>
       </c>
       <c r="D11" s="4">
         <v>460.48</v>

</xml_diff>